<commit_message>
Update inventory exposure simulation with enhanced analysis and presentation plots
</commit_message>
<xml_diff>
--- a/inventory exposure sim/uniswap_v3_lp_analysis_r1.0001.xlsx
+++ b/inventory exposure sim/uniswap_v3_lp_analysis_r1.0001.xlsx
@@ -518,13 +518,13 @@
         <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0004081853396176172</v>
+        <v>-0.0004081820073276177</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0004081853395954127</v>
+        <v>-0.0004040162853602425</v>
       </c>
       <c r="H3" t="n">
-        <v>99.9999999945602</v>
+        <v>98.97944497979019</v>
       </c>
     </row>
     <row r="4">
@@ -544,13 +544,13 @@
         <v>97.95888787025493</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0004081836734615152</v>
+        <v>-0.0004081803412270268</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0004040179176545422</v>
+        <v>-0.0003956832757334716</v>
       </c>
       <c r="H4" t="n">
-        <v>98.97944085522917</v>
+        <v>96.93834704141118</v>
       </c>
     </row>
     <row r="5">
@@ -570,13 +570,13 @@
         <v>95.91779605869726</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0004081820073498221</v>
+        <v>-0.0004081786751042316</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0003956848414032876</v>
+        <v>-0.0003873504153428797</v>
       </c>
       <c r="H5" t="n">
-        <v>96.93833492865743</v>
+        <v>94.89726900700209</v>
       </c>
     </row>
     <row r="6">
@@ -596,13 +596,13 @@
         <v>93.87672405521994</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0004081803412159246</v>
+        <v>-0.000408177009014743</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0003873519157426841</v>
+        <v>-0.0003790177020901453</v>
       </c>
       <c r="H6" t="n">
-        <v>94.89724923762989</v>
+        <v>92.85621034977389</v>
       </c>
     </row>
     <row r="7">
@@ -622,13 +622,13 @@
         <v>91.83567134931158</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0004081786751042316</v>
+        <v>-0.0004081753429585611</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0003790191386521258</v>
+        <v>-0.0003706851338769468</v>
       </c>
       <c r="H7" t="n">
-        <v>92.85618327692899</v>
+        <v>90.81517055638993</v>
       </c>
     </row>
     <row r="8">
@@ -648,13 +648,13 @@
         <v>89.79463743048237</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0004081770090369474</v>
+        <v>-0.0004081736768690725</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0003706865079555755</v>
+        <v>-0.0003623527086715761</v>
       </c>
       <c r="H8" t="n">
-        <v>90.815136509078</v>
+        <v>88.77414914431287</v>
       </c>
     </row>
     <row r="9">
@@ -674,13 +674,13 @@
         <v>87.75362178869017</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0004081753429474588</v>
+        <v>-0.0004081720108239928</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0003623540216768362</v>
+        <v>-0.0003540204243090983</v>
       </c>
       <c r="H9" t="n">
-        <v>88.77410846531197</v>
+        <v>86.73314556635655</v>
       </c>
     </row>
     <row r="10">
@@ -700,13 +700,13 @@
         <v>85.71262391334506</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0004081736768801747</v>
+        <v>-0.0004081703447900153</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0003540216776176663</v>
+        <v>-0.0003456882788022142</v>
       </c>
       <c r="H10" t="n">
-        <v>86.73309859753512</v>
+        <v>84.69215934343656</v>
       </c>
     </row>
     <row r="11">
@@ -726,13 +726,13 @@
         <v>83.67164329430388</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0004081720108128906</v>
+        <v>-0.0004081686787782424</v>
       </c>
       <c r="G11" t="n">
-        <v>0.000345689473801869</v>
+        <v>-0.0003373562699637844</v>
       </c>
       <c r="H11" t="n">
-        <v>84.6921064267525</v>
+        <v>82.65118993784178</v>
       </c>
     </row>
     <row r="12">
@@ -752,13 +752,13 @@
         <v>81.6306794208749</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0004081703448122198</v>
+        <v>-0.0004081670127553672</v>
       </c>
       <c r="G12" t="n">
-        <v>0.000337357408053407</v>
+        <v>-0.0003290243957621009</v>
       </c>
       <c r="H12" t="n">
-        <v>82.65113140657228</v>
+        <v>80.61023685892519</v>
       </c>
     </row>
     <row r="13">
@@ -778,13 +778,13 @@
         <v>79.58973178338076</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0004081686787671401</v>
+        <v>-0.0004081653467546964</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0003290254783294699</v>
+        <v>-0.0003206926541432509</v>
       </c>
       <c r="H13" t="n">
-        <v>80.61017305964789</v>
+        <v>78.5692995971028</v>
       </c>
     </row>
     <row r="14">
@@ -804,13 +804,13 @@
         <v>77.5487998711683</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0004081670127442649</v>
+        <v>-0.0004081636807873323</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0003206936825872475</v>
+        <v>-0.0003123610429978108</v>
       </c>
       <c r="H14" t="n">
-        <v>78.56923087221078</v>
+        <v>76.52837763401146</v>
       </c>
     </row>
     <row r="15">
@@ -830,13 +830,13 @@
         <v>75.50788317402942</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0004081653467657986</v>
+        <v>-0.000408162014808866</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0003123620186951115</v>
+        <v>-0.0003040295601941523</v>
       </c>
       <c r="H15" t="n">
-        <v>76.52830431838248</v>
+        <v>74.48747045619204</v>
       </c>
     </row>
     <row r="16">
@@ -856,13 +856,13 @@
         <v>73.46698118205845</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0004081636807651279</v>
+        <v>-0.0004081603488526042</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0003040304845214337</v>
+        <v>-0.0002956982036450562</v>
       </c>
       <c r="H16" t="n">
-        <v>74.48739288892874</v>
+        <v>72.4465775463749</v>
       </c>
     </row>
     <row r="17">
@@ -882,13 +882,13 @@
         <v>71.42609338465694</v>
       </c>
       <c r="F17" t="n">
-        <v>0.000408162014808866</v>
+        <v>-0.0004081586829296491</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0002956990780234037</v>
+        <v>-0.0002873669714076321</v>
       </c>
       <c r="H17" t="n">
-        <v>72.4464960713881</v>
+        <v>70.40569842713923</v>
       </c>
     </row>
     <row r="18">
@@ -908,13 +908,13 @@
         <v>69.38521927181233</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0004081603488748087</v>
+        <v>-0.0004081570169844895</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0002873677972026201</v>
+        <v>-0.0002790358612392296</v>
       </c>
       <c r="H18" t="n">
-        <v>70.40561338082397</v>
+        <v>68.36483255899368</v>
       </c>
     </row>
     <row r="19">
@@ -934,13 +934,13 @@
         <v>67.34435833338679</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0004081586828963424</v>
+        <v>-0.0004081553510615343</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0002790366398386368</v>
+        <v>-0.0002707048710970383</v>
       </c>
       <c r="H19" t="n">
-        <v>68.36474428488442</v>
+        <v>66.32397943405287</v>
       </c>
     </row>
     <row r="20">
@@ -960,13 +960,13 @@
         <v>65.30351005925918</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0004081570169844895</v>
+        <v>-0.0004081536851829881</v>
       </c>
       <c r="G20" t="n">
-        <v>0.000270705603910848</v>
+        <v>-0.0002623739989826568</v>
       </c>
       <c r="H20" t="n">
-        <v>66.32388826997311</v>
+        <v>64.28313855968892</v>
       </c>
     </row>
     <row r="21">
@@ -986,13 +986,13 @@
         <v>63.26267393918218</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0004081553510726366</v>
+        <v>-0.0004081520192711352</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0002623746873764432</v>
+        <v>-0.0002540432426978434</v>
       </c>
       <c r="H21" t="n">
-        <v>64.28304484724254</v>
+        <v>62.24230940998544</v>
       </c>
     </row>
     <row r="22">
@@ -1012,13 +1012,13 @@
         <v>61.22184946320849</v>
       </c>
       <c r="F22" t="n">
-        <v>0.0004081536851607837</v>
+        <v>-0.0004081503534036912</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0002540438880815898</v>
+        <v>-0.00024571260021089</v>
       </c>
       <c r="H22" t="n">
-        <v>62.24221348914553</v>
+        <v>60.20149147533921</v>
       </c>
     </row>
     <row r="23">
@@ -1038,13 +1038,13 @@
         <v>59.18103612112176</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0004081520192711352</v>
+        <v>-0.0004081486875362472</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0002457132039612731</v>
+        <v>-0.0002373820694345774</v>
       </c>
       <c r="H23" t="n">
-        <v>60.20139368661211</v>
+        <v>58.16068425149493</v>
       </c>
     </row>
     <row r="24">
@@ -1064,13 +1064,13 @@
         <v>57.14023340286265</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0004081503534036912</v>
+        <v>-0.0004081470217132122</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0002373826329282736</v>
+        <v>-0.0002290516483149929</v>
       </c>
       <c r="H24" t="n">
-        <v>58.16058492873199</v>
+        <v>56.11988722924895</v>
       </c>
     </row>
     <row r="25">
@@ -1090,13 +1090,13 @@
         <v>55.09944079838617</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0004081486875584517</v>
+        <v>-0.0004081453558568704</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0002290521729619854</v>
+        <v>-0.0002207213346983039</v>
       </c>
       <c r="H25" t="n">
-        <v>56.11978672090731</v>
+        <v>54.07909989197748</v>
       </c>
     </row>
     <row r="26">
@@ -1116,13 +1116,13 @@
         <v>53.05865779751918</v>
       </c>
       <c r="F26" t="n">
-        <v>0.0004081470216910077</v>
+        <v>-0.0004081436900449376</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0002207218218863716</v>
+        <v>-0.0002123911265750067</v>
       </c>
       <c r="H26" t="n">
-        <v>54.07899853633418</v>
+        <v>52.03832173703873</v>
       </c>
     </row>
     <row r="27">
@@ -1142,13 +1142,13 @@
         <v>51.01788389038636</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0004081453558679726</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0.0002123915776808261</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>52.0382198712389</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">

</xml_diff>